<commit_message>
Changes in .xlsx files. Moved graphs to the correct positions.
</commit_message>
<xml_diff>
--- a/Отчёт/EachGraphComparison - First.xlsx
+++ b/Отчёт/EachGraphComparison - First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Construction and analysis of algorithms\SortAlgorithms\Отчёт\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{095CDD35-F521-4DA1-96C6-6B58F43B9CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B275AA8C-E32F-47BC-897D-1C105DC4B268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23002,8 +23002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U28" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AX81" sqref="AX81"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AY82" sqref="AY82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>